<commit_message>
update xl file, add batch script examples
</commit_message>
<xml_diff>
--- a/mini_bam_v1/Exercice identification des évènements sur IGV.xlsx
+++ b/mini_bam_v1/Exercice identification des évènements sur IGV.xlsx
@@ -835,9 +835,15 @@
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
       <formula1>difficulte_A</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E7">
+      <formula1>difficulte_B</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E10">
+      <formula1>difficulte_C</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>